<commit_message>
added perfect, missed counts
</commit_message>
<xml_diff>
--- a/error_rankings/biodivner/new_categories_full_prompts_small_models_error_category_ranking.xlsx
+++ b/error_rankings/biodivner/new_categories_full_prompts_small_models_error_category_ranking.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,7 +466,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> QUALITY</t>
+          <t>MATERIAL</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -479,7 +479,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>MATERIAL</t>
+          <t>MATTERMATTER</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -492,7 +492,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>MATTERMATTER</t>
+          <t>ORGANSIM</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -505,7 +505,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>ORGANSIM</t>
+          <t>PROTEIN</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -518,26 +518,13 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>PROTEIN</t>
+          <t>TREE</t>
         </is>
       </c>
       <c r="B7" t="n">
         <v>0.08333333333333333</v>
       </c>
       <c r="C7" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>TREE</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>0.08333333333333333</v>
-      </c>
-      <c r="C8" t="n">
         <v>2</v>
       </c>
     </row>

</xml_diff>